<commit_message>
data set balancing - ACER
</commit_message>
<xml_diff>
--- a/Code/fypDS.xlsx
+++ b/Code/fypDS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Documents\GitHub\Undergraduate-Final-Year-Project-\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Documents\GitHub\Undergraduate-Final-Year-Project-\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{150711A9-381B-41C8-916E-D353435840A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55350289-1033-4E34-93B1-D1AD16620163}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11355" xr2:uid="{6959E88D-E4AE-4485-A512-4E79A32FE670}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6959E88D-E4AE-4485-A512-4E79A32FE670}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="325">
   <si>
     <t>hate</t>
   </si>
@@ -919,6 +919,99 @@
   </si>
   <si>
     <t>COM119</t>
+  </si>
+  <si>
+    <t>ammige hinawama thiyena lassana puthek</t>
+  </si>
+  <si>
+    <t>COM120</t>
+  </si>
+  <si>
+    <t>COM121</t>
+  </si>
+  <si>
+    <t>COM122</t>
+  </si>
+  <si>
+    <t>COM123</t>
+  </si>
+  <si>
+    <t>COM124</t>
+  </si>
+  <si>
+    <t>COM125</t>
+  </si>
+  <si>
+    <t>COM126</t>
+  </si>
+  <si>
+    <t>COM127</t>
+  </si>
+  <si>
+    <t>COM128</t>
+  </si>
+  <si>
+    <t>COM129</t>
+  </si>
+  <si>
+    <t>COM130</t>
+  </si>
+  <si>
+    <t>COM131</t>
+  </si>
+  <si>
+    <t>COM132</t>
+  </si>
+  <si>
+    <t>COM133</t>
+  </si>
+  <si>
+    <t>COM134</t>
+  </si>
+  <si>
+    <t>COM135</t>
+  </si>
+  <si>
+    <t>COM136</t>
+  </si>
+  <si>
+    <t>COM137</t>
+  </si>
+  <si>
+    <t>COM138</t>
+  </si>
+  <si>
+    <t>COM139</t>
+  </si>
+  <si>
+    <t>Budu saranai puthe oyata</t>
+  </si>
+  <si>
+    <t>Carima panditayek wei mu issarahata</t>
+  </si>
+  <si>
+    <t>carima</t>
+  </si>
+  <si>
+    <t>Ane me pakayage nambar Eka nadda</t>
+  </si>
+  <si>
+    <t>pakayage</t>
+  </si>
+  <si>
+    <t>Pissu pakayek muta riport gahapalla okkom ekathu.wela</t>
+  </si>
+  <si>
+    <t>pakayek</t>
+  </si>
+  <si>
+    <t>Waddek</t>
+  </si>
+  <si>
+    <t>Ithin laccna pacyo dn kt whn plyn</t>
+  </si>
+  <si>
+    <t>pacyo</t>
   </si>
 </sst>
 </file>
@@ -1306,10 +1399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABD71A72-8387-4123-B42C-650C0C79B145}">
-  <dimension ref="A1:I120"/>
+  <dimension ref="A1:I140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="F125" sqref="F125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3855,7 +3948,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>291</v>
       </c>
@@ -3871,8 +3964,11 @@
       <c r="E118">
         <v>0</v>
       </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F118" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>292</v>
       </c>
@@ -3888,21 +3984,391 @@
       <c r="E119">
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F119" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>293</v>
       </c>
       <c r="B120">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C120">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D120">
         <v>0</v>
       </c>
       <c r="E120">
+        <v>1</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="G120" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>295</v>
+      </c>
+      <c r="B121">
+        <v>0</v>
+      </c>
+      <c r="C121">
+        <v>1</v>
+      </c>
+      <c r="D121">
+        <v>0</v>
+      </c>
+      <c r="E121">
+        <v>1</v>
+      </c>
+      <c r="F121" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="G121" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>296</v>
+      </c>
+      <c r="B122">
+        <v>0</v>
+      </c>
+      <c r="C122">
+        <v>0</v>
+      </c>
+      <c r="D122">
+        <v>0</v>
+      </c>
+      <c r="E122">
+        <v>0</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="G122" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>297</v>
+      </c>
+      <c r="B123">
+        <v>0</v>
+      </c>
+      <c r="C123">
+        <v>0</v>
+      </c>
+      <c r="D123">
+        <v>0</v>
+      </c>
+      <c r="E123">
+        <v>0</v>
+      </c>
+      <c r="F123" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>298</v>
+      </c>
+      <c r="B124">
+        <v>0</v>
+      </c>
+      <c r="C124">
+        <v>1</v>
+      </c>
+      <c r="D124">
+        <v>0</v>
+      </c>
+      <c r="E124">
+        <v>1</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="G124" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>299</v>
+      </c>
+      <c r="B125">
+        <v>0</v>
+      </c>
+      <c r="C125">
+        <v>0</v>
+      </c>
+      <c r="D125">
+        <v>0</v>
+      </c>
+      <c r="E125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>300</v>
+      </c>
+      <c r="B126">
+        <v>0</v>
+      </c>
+      <c r="C126">
+        <v>0</v>
+      </c>
+      <c r="D126">
+        <v>0</v>
+      </c>
+      <c r="E126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>301</v>
+      </c>
+      <c r="B127">
+        <v>0</v>
+      </c>
+      <c r="C127">
+        <v>0</v>
+      </c>
+      <c r="D127">
+        <v>0</v>
+      </c>
+      <c r="E127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>302</v>
+      </c>
+      <c r="B128">
+        <v>0</v>
+      </c>
+      <c r="C128">
+        <v>0</v>
+      </c>
+      <c r="D128">
+        <v>0</v>
+      </c>
+      <c r="E128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>303</v>
+      </c>
+      <c r="B129">
+        <v>0</v>
+      </c>
+      <c r="C129">
+        <v>0</v>
+      </c>
+      <c r="D129">
+        <v>0</v>
+      </c>
+      <c r="E129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>304</v>
+      </c>
+      <c r="B130">
+        <v>0</v>
+      </c>
+      <c r="C130">
+        <v>0</v>
+      </c>
+      <c r="D130">
+        <v>0</v>
+      </c>
+      <c r="E130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>305</v>
+      </c>
+      <c r="B131">
+        <v>0</v>
+      </c>
+      <c r="C131">
+        <v>0</v>
+      </c>
+      <c r="D131">
+        <v>0</v>
+      </c>
+      <c r="E131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>306</v>
+      </c>
+      <c r="B132">
+        <v>0</v>
+      </c>
+      <c r="C132">
+        <v>0</v>
+      </c>
+      <c r="D132">
+        <v>0</v>
+      </c>
+      <c r="E132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>307</v>
+      </c>
+      <c r="B133">
+        <v>0</v>
+      </c>
+      <c r="C133">
+        <v>0</v>
+      </c>
+      <c r="D133">
+        <v>0</v>
+      </c>
+      <c r="E133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>308</v>
+      </c>
+      <c r="B134">
+        <v>0</v>
+      </c>
+      <c r="C134">
+        <v>0</v>
+      </c>
+      <c r="D134">
+        <v>0</v>
+      </c>
+      <c r="E134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>309</v>
+      </c>
+      <c r="B135">
+        <v>0</v>
+      </c>
+      <c r="C135">
+        <v>0</v>
+      </c>
+      <c r="D135">
+        <v>0</v>
+      </c>
+      <c r="E135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>310</v>
+      </c>
+      <c r="B136">
+        <v>0</v>
+      </c>
+      <c r="C136">
+        <v>0</v>
+      </c>
+      <c r="D136">
+        <v>0</v>
+      </c>
+      <c r="E136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>311</v>
+      </c>
+      <c r="B137">
+        <v>0</v>
+      </c>
+      <c r="C137">
+        <v>0</v>
+      </c>
+      <c r="D137">
+        <v>0</v>
+      </c>
+      <c r="E137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>312</v>
+      </c>
+      <c r="B138">
+        <v>0</v>
+      </c>
+      <c r="C138">
+        <v>0</v>
+      </c>
+      <c r="D138">
+        <v>0</v>
+      </c>
+      <c r="E138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>313</v>
+      </c>
+      <c r="B139">
+        <v>0</v>
+      </c>
+      <c r="C139">
+        <v>0</v>
+      </c>
+      <c r="D139">
+        <v>0</v>
+      </c>
+      <c r="E139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>314</v>
+      </c>
+      <c r="B140">
+        <v>0</v>
+      </c>
+      <c r="C140">
+        <v>0</v>
+      </c>
+      <c r="D140">
+        <v>0</v>
+      </c>
+      <c r="E140">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update documents - ACER
</commit_message>
<xml_diff>
--- a/Code/fypDS.xlsx
+++ b/Code/fypDS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Documents\GitHub\Undergraduate-Final-Year-Project-\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55350289-1033-4E34-93B1-D1AD16620163}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0BCA376-6E72-40C6-9CAD-84186BD149FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6959E88D-E4AE-4485-A512-4E79A32FE670}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="371">
   <si>
     <t>hate</t>
   </si>
@@ -1012,6 +1012,144 @@
   </si>
   <si>
     <t>pacyo</t>
+  </si>
+  <si>
+    <t>Wetenna epa malli negitapan</t>
+  </si>
+  <si>
+    <t>Ub nm gmmc bn</t>
+  </si>
+  <si>
+    <t>Oya gamma digatama tiyagamu. Salenna epa aiye. Hadawathinma suba pathanawa</t>
+  </si>
+  <si>
+    <t>Ohoma hinawela santhosen inna!</t>
+  </si>
+  <si>
+    <t>Adarei machan Supiri charithayak!!</t>
+  </si>
+  <si>
+    <t>Subadawasak wewa</t>
+  </si>
+  <si>
+    <t>Onna ohoma hina wela hitapn kollo</t>
+  </si>
+  <si>
+    <t>Bhkpn</t>
+  </si>
+  <si>
+    <t>Munge munawalwalinma penawa mandabuddika gobbayo set ekak kiyala</t>
+  </si>
+  <si>
+    <t>niyamaiii harima lassanai sweet ape Ashen adareiiiii hamadaamath satutin parissamin Inna hode bs</t>
+  </si>
+  <si>
+    <t>Velavakata hithenne nadda lankawe minissunt kochchara hoda krath . Ee gollongen hodak ahanna venne nha kiyla</t>
+  </si>
+  <si>
+    <t>Wipathakne wela thiyenne</t>
+  </si>
+  <si>
+    <t>Pissu huththek</t>
+  </si>
+  <si>
+    <t>huththek</t>
+  </si>
+  <si>
+    <t>Ayeth Hitiya Wge Imu</t>
+  </si>
+  <si>
+    <t>Lassanai</t>
+  </si>
+  <si>
+    <t>COM140</t>
+  </si>
+  <si>
+    <t>COM141</t>
+  </si>
+  <si>
+    <t>COM142</t>
+  </si>
+  <si>
+    <t>COM143</t>
+  </si>
+  <si>
+    <t>COM144</t>
+  </si>
+  <si>
+    <t>COM145</t>
+  </si>
+  <si>
+    <t>COM146</t>
+  </si>
+  <si>
+    <t>COM147</t>
+  </si>
+  <si>
+    <t>COM148</t>
+  </si>
+  <si>
+    <t>COM149</t>
+  </si>
+  <si>
+    <t>COM150</t>
+  </si>
+  <si>
+    <t>COM151</t>
+  </si>
+  <si>
+    <t>COM152</t>
+  </si>
+  <si>
+    <t>COM153</t>
+  </si>
+  <si>
+    <t>COM154</t>
+  </si>
+  <si>
+    <t>COM155</t>
+  </si>
+  <si>
+    <t>COM156</t>
+  </si>
+  <si>
+    <t>COM157</t>
+  </si>
+  <si>
+    <t>COM158</t>
+  </si>
+  <si>
+    <t>COM159</t>
+  </si>
+  <si>
+    <t>Gong ponnya</t>
+  </si>
+  <si>
+    <t>ponnaya</t>
+  </si>
+  <si>
+    <t>Toilet eke idagenath video karala daapan fb ekata uba thawath femous vei</t>
+  </si>
+  <si>
+    <t>Oyaata kohomadha</t>
+  </si>
+  <si>
+    <t>Supiri song eka</t>
+  </si>
+  <si>
+    <t>Thawa wayasa thiyenawa .issarahata api illamu .budusaranai mall</t>
+  </si>
+  <si>
+    <t>Sudu thaththiyek</t>
+  </si>
+  <si>
+    <t>Okage mole pedena kan masaj karapan</t>
+  </si>
+  <si>
+    <t>Jaya wewa</t>
+  </si>
+  <si>
+    <t>Konde kapanakota hollanda epa manussayo.</t>
   </si>
 </sst>
 </file>
@@ -1399,15 +1537,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABD71A72-8387-4123-B42C-650C0C79B145}">
-  <dimension ref="A1:I140"/>
+  <dimension ref="A1:I160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="F125" sqref="F125"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="F149" sqref="F149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="99.28515625" customWidth="1"/>
+    <col min="6" max="6" width="108.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -2328,7 +2466,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>218</v>
       </c>
@@ -4100,7 +4238,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>299</v>
       </c>
@@ -4116,8 +4254,11 @@
       <c r="E125">
         <v>0</v>
       </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F125" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>300</v>
       </c>
@@ -4133,8 +4274,11 @@
       <c r="E126">
         <v>0</v>
       </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F126" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>301</v>
       </c>
@@ -4150,8 +4294,11 @@
       <c r="E127">
         <v>0</v>
       </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F127" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>302</v>
       </c>
@@ -4167,8 +4314,11 @@
       <c r="E128">
         <v>0</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F128" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>303</v>
       </c>
@@ -4184,8 +4334,11 @@
       <c r="E129">
         <v>0</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F129" s="1" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>304</v>
       </c>
@@ -4201,8 +4354,11 @@
       <c r="E130">
         <v>0</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F130" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>305</v>
       </c>
@@ -4218,8 +4374,11 @@
       <c r="E131">
         <v>0</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F131" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>306</v>
       </c>
@@ -4227,21 +4386,27 @@
         <v>0</v>
       </c>
       <c r="C132">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D132">
         <v>0</v>
       </c>
       <c r="E132">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F132" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="G132" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>307</v>
       </c>
       <c r="B133">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C133">
         <v>0</v>
@@ -4250,10 +4415,13 @@
         <v>0</v>
       </c>
       <c r="E133">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F133" s="1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>308</v>
       </c>
@@ -4269,8 +4437,11 @@
       <c r="E134">
         <v>0</v>
       </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F134" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>309</v>
       </c>
@@ -4286,8 +4457,11 @@
       <c r="E135">
         <v>0</v>
       </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F135" s="1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>310</v>
       </c>
@@ -4303,8 +4477,11 @@
       <c r="E136">
         <v>0</v>
       </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F136" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>311</v>
       </c>
@@ -4312,16 +4489,22 @@
         <v>0</v>
       </c>
       <c r="C137">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D137">
         <v>0</v>
       </c>
       <c r="E137">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="G137" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>312</v>
       </c>
@@ -4337,8 +4520,11 @@
       <c r="E138">
         <v>0</v>
       </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F138" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>313</v>
       </c>
@@ -4354,21 +4540,394 @@
       <c r="E139">
         <v>0</v>
       </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F139" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>314</v>
       </c>
       <c r="B140">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C140">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D140">
         <v>0</v>
       </c>
       <c r="E140">
+        <v>1</v>
+      </c>
+      <c r="F140" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="G140" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>341</v>
+      </c>
+      <c r="B141">
+        <v>1</v>
+      </c>
+      <c r="C141">
+        <v>0</v>
+      </c>
+      <c r="D141">
+        <v>0</v>
+      </c>
+      <c r="E141">
+        <v>1</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>342</v>
+      </c>
+      <c r="B142">
+        <v>0</v>
+      </c>
+      <c r="C142">
+        <v>0</v>
+      </c>
+      <c r="D142">
+        <v>0</v>
+      </c>
+      <c r="E142">
+        <v>0</v>
+      </c>
+      <c r="F142" s="1" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>343</v>
+      </c>
+      <c r="B143">
+        <v>0</v>
+      </c>
+      <c r="C143">
+        <v>0</v>
+      </c>
+      <c r="D143">
+        <v>0</v>
+      </c>
+      <c r="E143">
+        <v>0</v>
+      </c>
+      <c r="F143" s="1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>344</v>
+      </c>
+      <c r="B144">
+        <v>0</v>
+      </c>
+      <c r="C144">
+        <v>0</v>
+      </c>
+      <c r="D144">
+        <v>0</v>
+      </c>
+      <c r="E144">
+        <v>0</v>
+      </c>
+      <c r="F144" s="1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>345</v>
+      </c>
+      <c r="B145">
+        <v>0</v>
+      </c>
+      <c r="C145">
+        <v>0</v>
+      </c>
+      <c r="D145">
+        <v>0</v>
+      </c>
+      <c r="E145">
+        <v>0</v>
+      </c>
+      <c r="F145" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>346</v>
+      </c>
+      <c r="B146">
+        <v>1</v>
+      </c>
+      <c r="C146">
+        <v>0</v>
+      </c>
+      <c r="D146">
+        <v>0</v>
+      </c>
+      <c r="E146">
+        <v>1</v>
+      </c>
+      <c r="F146" s="1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>347</v>
+      </c>
+      <c r="B147">
+        <v>0</v>
+      </c>
+      <c r="C147">
+        <v>0</v>
+      </c>
+      <c r="D147">
+        <v>0</v>
+      </c>
+      <c r="E147">
+        <v>0</v>
+      </c>
+      <c r="F147" s="1" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>348</v>
+      </c>
+      <c r="B148">
+        <v>0</v>
+      </c>
+      <c r="C148">
+        <v>0</v>
+      </c>
+      <c r="D148">
+        <v>0</v>
+      </c>
+      <c r="E148">
+        <v>0</v>
+      </c>
+      <c r="F148" s="1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>349</v>
+      </c>
+      <c r="B149">
+        <v>0</v>
+      </c>
+      <c r="C149">
+        <v>0</v>
+      </c>
+      <c r="D149">
+        <v>0</v>
+      </c>
+      <c r="E149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>350</v>
+      </c>
+      <c r="B150">
+        <v>0</v>
+      </c>
+      <c r="C150">
+        <v>0</v>
+      </c>
+      <c r="D150">
+        <v>0</v>
+      </c>
+      <c r="E150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>351</v>
+      </c>
+      <c r="B151">
+        <v>0</v>
+      </c>
+      <c r="C151">
+        <v>0</v>
+      </c>
+      <c r="D151">
+        <v>0</v>
+      </c>
+      <c r="E151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>352</v>
+      </c>
+      <c r="B152">
+        <v>0</v>
+      </c>
+      <c r="C152">
+        <v>0</v>
+      </c>
+      <c r="D152">
+        <v>0</v>
+      </c>
+      <c r="E152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>353</v>
+      </c>
+      <c r="B153">
+        <v>0</v>
+      </c>
+      <c r="C153">
+        <v>0</v>
+      </c>
+      <c r="D153">
+        <v>0</v>
+      </c>
+      <c r="E153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>354</v>
+      </c>
+      <c r="B154">
+        <v>0</v>
+      </c>
+      <c r="C154">
+        <v>0</v>
+      </c>
+      <c r="D154">
+        <v>0</v>
+      </c>
+      <c r="E154">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>355</v>
+      </c>
+      <c r="B155">
+        <v>0</v>
+      </c>
+      <c r="C155">
+        <v>0</v>
+      </c>
+      <c r="D155">
+        <v>0</v>
+      </c>
+      <c r="E155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>356</v>
+      </c>
+      <c r="B156">
+        <v>0</v>
+      </c>
+      <c r="C156">
+        <v>0</v>
+      </c>
+      <c r="D156">
+        <v>0</v>
+      </c>
+      <c r="E156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>357</v>
+      </c>
+      <c r="B157">
+        <v>0</v>
+      </c>
+      <c r="C157">
+        <v>0</v>
+      </c>
+      <c r="D157">
+        <v>0</v>
+      </c>
+      <c r="E157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>358</v>
+      </c>
+      <c r="B158">
+        <v>0</v>
+      </c>
+      <c r="C158">
+        <v>0</v>
+      </c>
+      <c r="D158">
+        <v>0</v>
+      </c>
+      <c r="E158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>359</v>
+      </c>
+      <c r="B159">
+        <v>0</v>
+      </c>
+      <c r="C159">
+        <v>0</v>
+      </c>
+      <c r="D159">
+        <v>0</v>
+      </c>
+      <c r="E159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>360</v>
+      </c>
+      <c r="B160">
+        <v>0</v>
+      </c>
+      <c r="C160">
+        <v>0</v>
+      </c>
+      <c r="D160">
+        <v>0</v>
+      </c>
+      <c r="E160">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Code changing to check probability - ACER
</commit_message>
<xml_diff>
--- a/Code/fypDS.xlsx
+++ b/Code/fypDS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Documents\GitHub\Undergraduate-Final-Year-Project-\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0BCA376-6E72-40C6-9CAD-84186BD149FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27544193-ABED-4B95-B7E3-0D4EF41D1E8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6959E88D-E4AE-4485-A512-4E79A32FE670}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="394">
   <si>
     <t>hate</t>
   </si>
@@ -1150,6 +1150,75 @@
   </si>
   <si>
     <t>Konde kapanakota hollanda epa manussayo.</t>
+  </si>
+  <si>
+    <t>kalakanni ballo okkoma marila yanna one than than wala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hati balapn mekige. </t>
+  </si>
+  <si>
+    <t>paththini amma wage hitiyata wate yana hoda badu thamai mewa</t>
+  </si>
+  <si>
+    <t>baduwak thamai oyath hoda wada karata</t>
+  </si>
+  <si>
+    <t>padurugane lagala hada gatta lamai thamai oya ellan inne. Patta wesiyo</t>
+  </si>
+  <si>
+    <t>wesiyo</t>
+  </si>
+  <si>
+    <t>patta wesiyo</t>
+  </si>
+  <si>
+    <t>Ballonta jathaka wechcha un</t>
+  </si>
+  <si>
+    <t>marila palayan</t>
+  </si>
+  <si>
+    <t>kala kanni okkoma marila palayan</t>
+  </si>
+  <si>
+    <t>wedi thiyala marala yanne ubalage pawula pitin</t>
+  </si>
+  <si>
+    <t>COM160</t>
+  </si>
+  <si>
+    <t>COM161</t>
+  </si>
+  <si>
+    <t>COM162</t>
+  </si>
+  <si>
+    <t>COM163</t>
+  </si>
+  <si>
+    <t>COM164</t>
+  </si>
+  <si>
+    <t>COM165</t>
+  </si>
+  <si>
+    <t>COM166</t>
+  </si>
+  <si>
+    <t>COM167</t>
+  </si>
+  <si>
+    <t>COM168</t>
+  </si>
+  <si>
+    <t>COM169</t>
+  </si>
+  <si>
+    <t>mewa hora upadi kada</t>
+  </si>
+  <si>
+    <t>wal ballo ubala okkma</t>
   </si>
 </sst>
 </file>
@@ -1537,10 +1606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABD71A72-8387-4123-B42C-650C0C79B145}">
-  <dimension ref="A1:I160"/>
+  <dimension ref="A1:I170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="F149" sqref="F149"/>
+    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
+      <selection activeCell="M139" sqref="M139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4647,7 +4716,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="145" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>345</v>
       </c>
@@ -4667,7 +4736,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="146" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>346</v>
       </c>
@@ -4687,7 +4756,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="147" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>347</v>
       </c>
@@ -4707,7 +4776,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="148" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>348</v>
       </c>
@@ -4727,12 +4796,12 @@
         <v>370</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>349</v>
       </c>
       <c r="B149">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C149">
         <v>0</v>
@@ -4741,15 +4810,18 @@
         <v>0</v>
       </c>
       <c r="E149">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F149" s="1" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>350</v>
       </c>
       <c r="B150">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C150">
         <v>0</v>
@@ -4758,15 +4830,18 @@
         <v>0</v>
       </c>
       <c r="E150">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F150" s="1" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>351</v>
       </c>
       <c r="B151">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C151">
         <v>0</v>
@@ -4775,15 +4850,18 @@
         <v>0</v>
       </c>
       <c r="E151">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F151" s="1" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>352</v>
       </c>
       <c r="B152">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C152">
         <v>0</v>
@@ -4792,32 +4870,44 @@
         <v>0</v>
       </c>
       <c r="E152">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F152" s="1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>353</v>
       </c>
       <c r="B153">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C153">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D153">
         <v>0</v>
       </c>
       <c r="E153">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F153" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="G153" t="s">
+        <v>376</v>
+      </c>
+      <c r="H153" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>354</v>
       </c>
       <c r="B154">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C154">
         <v>0</v>
@@ -4826,15 +4916,18 @@
         <v>0</v>
       </c>
       <c r="E154">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F154" s="1" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>355</v>
       </c>
       <c r="B155">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C155">
         <v>0</v>
@@ -4843,15 +4936,18 @@
         <v>0</v>
       </c>
       <c r="E155">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F155" s="1" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>356</v>
       </c>
       <c r="B156">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C156">
         <v>0</v>
@@ -4860,15 +4956,18 @@
         <v>0</v>
       </c>
       <c r="E156">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F156" s="1" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>357</v>
       </c>
       <c r="B157">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C157">
         <v>0</v>
@@ -4877,15 +4976,18 @@
         <v>0</v>
       </c>
       <c r="E157">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F157" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>358</v>
       </c>
       <c r="B158">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C158">
         <v>0</v>
@@ -4894,15 +4996,18 @@
         <v>0</v>
       </c>
       <c r="E158">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F158" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>359</v>
       </c>
       <c r="B159">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C159">
         <v>0</v>
@@ -4911,10 +5016,13 @@
         <v>0</v>
       </c>
       <c r="E159">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F159" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>360</v>
       </c>
@@ -4928,6 +5036,176 @@
         <v>0</v>
       </c>
       <c r="E160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>382</v>
+      </c>
+      <c r="B161">
+        <v>0</v>
+      </c>
+      <c r="C161">
+        <v>0</v>
+      </c>
+      <c r="D161">
+        <v>0</v>
+      </c>
+      <c r="E161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>383</v>
+      </c>
+      <c r="B162">
+        <v>0</v>
+      </c>
+      <c r="C162">
+        <v>0</v>
+      </c>
+      <c r="D162">
+        <v>0</v>
+      </c>
+      <c r="E162">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>384</v>
+      </c>
+      <c r="B163">
+        <v>0</v>
+      </c>
+      <c r="C163">
+        <v>0</v>
+      </c>
+      <c r="D163">
+        <v>0</v>
+      </c>
+      <c r="E163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>385</v>
+      </c>
+      <c r="B164">
+        <v>0</v>
+      </c>
+      <c r="C164">
+        <v>0</v>
+      </c>
+      <c r="D164">
+        <v>0</v>
+      </c>
+      <c r="E164">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>386</v>
+      </c>
+      <c r="B165">
+        <v>0</v>
+      </c>
+      <c r="C165">
+        <v>0</v>
+      </c>
+      <c r="D165">
+        <v>0</v>
+      </c>
+      <c r="E165">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>387</v>
+      </c>
+      <c r="B166">
+        <v>0</v>
+      </c>
+      <c r="C166">
+        <v>0</v>
+      </c>
+      <c r="D166">
+        <v>0</v>
+      </c>
+      <c r="E166">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>388</v>
+      </c>
+      <c r="B167">
+        <v>0</v>
+      </c>
+      <c r="C167">
+        <v>0</v>
+      </c>
+      <c r="D167">
+        <v>0</v>
+      </c>
+      <c r="E167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>389</v>
+      </c>
+      <c r="B168">
+        <v>0</v>
+      </c>
+      <c r="C168">
+        <v>0</v>
+      </c>
+      <c r="D168">
+        <v>0</v>
+      </c>
+      <c r="E168">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>390</v>
+      </c>
+      <c r="B169">
+        <v>0</v>
+      </c>
+      <c r="C169">
+        <v>0</v>
+      </c>
+      <c r="D169">
+        <v>0</v>
+      </c>
+      <c r="E169">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>391</v>
+      </c>
+      <c r="B170">
+        <v>0</v>
+      </c>
+      <c r="C170">
+        <v>0</v>
+      </c>
+      <c r="D170">
+        <v>0</v>
+      </c>
+      <c r="E170">
         <v>0</v>
       </c>
     </row>

</xml_diff>